<commit_message>
ajuste de excel de usuarios conectados
</commit_message>
<xml_diff>
--- a/docs/formatos/ListadoUsuariosConectados.xlsx
+++ b/docs/formatos/ListadoUsuariosConectados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubicación</t>
   </si>
 </sst>
 </file>
@@ -203,11 +206,11 @@
   </sheetPr>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.42"/>
@@ -215,7 +218,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.23"/>
@@ -280,6 +283,9 @@
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>

</xml_diff>